<commit_message>
Atualização backlog e fluxogramas
</commit_message>
<xml_diff>
--- a/sprint_grupo7/TI/Backlog_TecnoSolo ATUALIZADO.xlsx
+++ b/sprint_grupo7/TI/Backlog_TecnoSolo ATUALIZADO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS\Desktop\aula\sptech\pesquisa e inovação\sprint_02\sprint_grupo7\TI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\OneDrive\Documentos\Pesquisa e inovação\sprint_01\sprint_grupo7\TI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E06F7E-F1C4-4B6D-A377-A4AAFBDB6893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E44B706-0B97-49A2-95D5-6789E69B399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1824" yWindow="0" windowWidth="21216" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="105">
   <si>
     <t>Descrição</t>
   </si>
@@ -313,6 +324,33 @@
   </si>
   <si>
     <t>Requisito</t>
+  </si>
+  <si>
+    <t>Documento com planejaento para uma parada no sistema planejada ou não.</t>
+  </si>
+  <si>
+    <t>Diagrama do passo a passo do suporte na ferramenta de HelpDesk</t>
+  </si>
+  <si>
+    <t>Ferramenta de helpDesk</t>
+  </si>
+  <si>
+    <t>Manual de instalação</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integração com API (Web Data Vis) </t>
+  </si>
+  <si>
+    <t>Integração API dashboard</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk FreshDesk para abrir tickets e chamados</t>
+  </si>
+  <si>
+    <t>Passo a passo para o cliente conseguir fazer instalação do sistema</t>
+  </si>
+  <si>
+    <t>Conexão com login e cadastro com banco de dados</t>
   </si>
 </sst>
 </file>
@@ -431,7 +469,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -790,11 +828,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -907,18 +973,6 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -987,32 +1041,14 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1032,16 +1068,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1054,6 +1081,63 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1260,29 +1344,10 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+      <border>
+        <bottom style="thin">
           <color theme="4" tint="-0.249977111117893"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </right>
-        <top/>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1312,17 +1377,36 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="-0.249977111117893"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1413,8 +1497,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requisitos" displayName="Requisitos" ref="A1:H36" headerRowDxfId="12" dataDxfId="10" totalsRowDxfId="8" headerRowBorderDxfId="11" tableBorderDxfId="9">
-  <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0100-000002000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requisitos" displayName="Requisitos" ref="A1:H39" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9">
+  <autoFilter ref="A1:H39" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1738,27 +1822,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DM36"/>
+  <dimension ref="A1:DM42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="10" width="10.28515625" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.6640625" customWidth="1"/>
+    <col min="9" max="10" width="10.33203125" customWidth="1"/>
+    <col min="16" max="16" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
         <v>95</v>
       </c>
@@ -1784,7 +1868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>52</v>
       </c>
@@ -1797,13 +1881,13 @@
       <c r="D2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="48" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="12">
         <v>5</v>
       </c>
-      <c r="G2" s="54">
+      <c r="G2" s="50">
         <v>5</v>
       </c>
       <c r="H2" s="35" t="s">
@@ -1817,7 +1901,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>29</v>
       </c>
@@ -1833,28 +1917,28 @@
       <c r="E3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="52">
+      <c r="F3" s="48">
         <v>8</v>
       </c>
       <c r="G3" s="32">
         <v>7</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="52" t="s">
         <v>43</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" s="60">
+      <c r="Q3" s="56">
         <f>SUM(F6,F8,F15)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="41" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="16" t="s">
@@ -1863,27 +1947,27 @@
       <c r="D4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="48">
         <v>5</v>
       </c>
       <c r="G4" s="7">
         <v>14</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="52" t="s">
         <v>43</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="Q4" s="61">
+      <c r="Q4" s="57">
         <f>SUM(F2,F3,F4,F5,F9,F11,F12,F24,F26,F29)</f>
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28" t="s">
         <v>9</v>
       </c>
@@ -1911,12 +1995,12 @@
       <c r="P5" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="Q5" s="61">
+      <c r="Q5" s="57">
         <f>SUM(F7,F10,F13,F16,F17,F18,F22,F19,F28)</f>
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>4</v>
       </c>
@@ -1935,7 +2019,7 @@
       <c r="F6" s="12">
         <v>8</v>
       </c>
-      <c r="G6" s="55">
+      <c r="G6" s="51">
         <v>3</v>
       </c>
       <c r="H6" s="35" t="s">
@@ -1945,16 +2029,16 @@
       <c r="P6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q6" s="62">
+      <c r="Q6" s="58">
         <f>SUM(F14,F20,F21,F23,F25,F27)</f>
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="50" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="15" t="s">
@@ -1977,12 +2061,12 @@
       </c>
       <c r="I7" s="2"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="63">
+      <c r="Q7" s="59">
         <f>SUM(Q3:Q6)</f>
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>34</v>
       </c>
@@ -2004,21 +2088,21 @@
       <c r="G8" s="32">
         <v>10</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="39" t="s">
         <v>41</v>
       </c>
       <c r="I8" s="2"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="64"/>
-    </row>
-    <row r="9" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="60"/>
+    </row>
+    <row r="9" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="44" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -2030,15 +2114,15 @@
       <c r="F9" s="11">
         <v>21</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="50">
         <v>11</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="39" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
         <v>57</v>
       </c>
@@ -2060,12 +2144,12 @@
       <c r="G10" s="7">
         <v>23</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="39" t="s">
         <v>41</v>
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
         <v>61</v>
       </c>
@@ -2092,26 +2176,26 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+    <row r="12" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="58">
+      <c r="F12" s="54">
         <v>5</v>
       </c>
-      <c r="G12" s="78">
+      <c r="G12" s="68">
         <v>28</v>
       </c>
       <c r="H12" s="35" t="s">
@@ -2119,7 +2203,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
         <v>31</v>
       </c>
@@ -2132,13 +2216,13 @@
       <c r="D13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="48" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="12">
         <v>5</v>
       </c>
-      <c r="G13" s="55">
+      <c r="G13" s="51">
         <v>8</v>
       </c>
       <c r="H13" s="35" t="s">
@@ -2146,14 +2230,14 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="45" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="21" t="s">
@@ -2172,7 +2256,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="31" t="s">
         <v>15</v>
       </c>
@@ -2198,7 +2282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
         <v>10</v>
       </c>
@@ -2217,40 +2301,40 @@
       <c r="F16" s="12">
         <v>8</v>
       </c>
-      <c r="G16" s="55">
+      <c r="G16" s="51">
         <v>16</v>
       </c>
       <c r="H16" s="35" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="69" t="s">
+    <row r="17" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="73" t="s">
+      <c r="E17" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="51">
+      <c r="F17" s="47">
         <v>13</v>
       </c>
-      <c r="G17" s="46">
+      <c r="G17" s="42">
         <v>20</v>
       </c>
-      <c r="H17" s="43" t="s">
+      <c r="H17" s="39" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:117" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:117" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
         <v>55</v>
       </c>
@@ -2260,10 +2344,10 @@
       <c r="C18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="48" t="s">
         <v>38</v>
       </c>
       <c r="F18" s="12">
@@ -2276,37 +2360,37 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:117" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+    <row r="19" spans="1:117" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="D19" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="49">
         <v>13</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="43">
         <v>13</v>
       </c>
-      <c r="H19" s="86" t="s">
+      <c r="H19" s="73" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:117" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:117" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="88" t="s">
+      <c r="B20" s="75" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -2328,7 +2412,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>36</v>
       </c>
@@ -2347,149 +2431,149 @@
       <c r="F21" s="12">
         <v>13</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="50">
         <v>9</v>
       </c>
       <c r="H21" s="35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:117" s="42" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
+    <row r="22" spans="1:117" s="38" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="44" t="s">
+      <c r="C22" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="44" t="s">
+      <c r="E22" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="40">
         <v>21</v>
       </c>
-      <c r="G22" s="87">
+      <c r="G22" s="74">
         <v>15</v>
       </c>
       <c r="H22" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="I22" s="59"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="59"/>
-      <c r="T22" s="59"/>
-      <c r="U22" s="59"/>
-      <c r="V22" s="59"/>
-      <c r="W22" s="59"/>
-      <c r="X22" s="59"/>
-      <c r="Y22" s="59"/>
-      <c r="Z22" s="59"/>
-      <c r="AA22" s="59"/>
-      <c r="AB22" s="59"/>
-      <c r="AC22" s="59"/>
-      <c r="AD22" s="59"/>
-      <c r="AE22" s="59"/>
-      <c r="AF22" s="59"/>
-      <c r="AG22" s="59"/>
-      <c r="AH22" s="59"/>
-      <c r="AI22" s="59"/>
-      <c r="AJ22" s="59"/>
-      <c r="AK22" s="59"/>
-      <c r="AL22" s="59"/>
-      <c r="AM22" s="59"/>
-      <c r="AN22" s="59"/>
-      <c r="AO22" s="59"/>
-      <c r="AP22" s="59"/>
-      <c r="AQ22" s="59"/>
-      <c r="AR22" s="59"/>
-      <c r="AS22" s="59"/>
-      <c r="AT22" s="59"/>
-      <c r="AU22" s="59"/>
-      <c r="AV22" s="59"/>
-      <c r="AW22" s="59"/>
-      <c r="AX22" s="59"/>
-      <c r="AY22" s="59"/>
-      <c r="AZ22" s="59"/>
-      <c r="BA22" s="59"/>
-      <c r="BB22" s="59"/>
-      <c r="BC22" s="59"/>
-      <c r="BD22" s="59"/>
-      <c r="BE22" s="59"/>
-      <c r="BF22" s="59"/>
-      <c r="BG22" s="59"/>
-      <c r="BH22" s="59"/>
-      <c r="BI22" s="59"/>
-      <c r="BJ22" s="59"/>
-      <c r="BK22" s="59"/>
-      <c r="BL22" s="59"/>
-      <c r="BM22" s="59"/>
-      <c r="BN22" s="59"/>
-      <c r="BO22" s="59"/>
-      <c r="BP22" s="59"/>
-      <c r="BQ22" s="59"/>
-      <c r="BR22" s="59"/>
-      <c r="BS22" s="59"/>
-      <c r="BT22" s="59"/>
-      <c r="BU22" s="59"/>
-      <c r="BV22" s="59"/>
-      <c r="BW22" s="59"/>
-      <c r="BX22" s="59"/>
-      <c r="BY22" s="59"/>
-      <c r="BZ22" s="59"/>
-      <c r="CA22" s="59"/>
-      <c r="CB22" s="59"/>
-      <c r="CC22" s="59"/>
-      <c r="CD22" s="59"/>
-      <c r="CE22" s="59"/>
-      <c r="CF22" s="59"/>
-      <c r="CG22" s="59"/>
-      <c r="CH22" s="59"/>
-      <c r="CI22" s="59"/>
-      <c r="CJ22" s="59"/>
-      <c r="CK22" s="59"/>
-      <c r="CL22" s="59"/>
-      <c r="CM22" s="59"/>
-      <c r="CN22" s="59"/>
-      <c r="CO22" s="59"/>
-      <c r="CP22" s="59"/>
-      <c r="CQ22" s="59"/>
-      <c r="CR22" s="59"/>
-      <c r="CS22" s="59"/>
-      <c r="CT22" s="59"/>
-      <c r="CU22" s="59"/>
-      <c r="CV22" s="59"/>
-      <c r="CW22" s="59"/>
-      <c r="CX22" s="59"/>
-      <c r="CY22" s="59"/>
-      <c r="CZ22" s="59"/>
-      <c r="DA22" s="59"/>
-      <c r="DB22" s="59"/>
-      <c r="DC22" s="59"/>
-      <c r="DD22" s="59"/>
-      <c r="DE22" s="59"/>
-      <c r="DF22" s="59"/>
-      <c r="DG22" s="59"/>
-      <c r="DH22" s="59"/>
-      <c r="DI22" s="59"/>
-      <c r="DJ22" s="59"/>
-      <c r="DK22" s="59"/>
-      <c r="DL22" s="59"/>
-      <c r="DM22" s="59"/>
-    </row>
-    <row r="23" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="55"/>
+      <c r="N22" s="55"/>
+      <c r="O22" s="55"/>
+      <c r="P22" s="55"/>
+      <c r="Q22" s="55"/>
+      <c r="R22" s="55"/>
+      <c r="S22" s="55"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="55"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="55"/>
+      <c r="X22" s="55"/>
+      <c r="Y22" s="55"/>
+      <c r="Z22" s="55"/>
+      <c r="AA22" s="55"/>
+      <c r="AB22" s="55"/>
+      <c r="AC22" s="55"/>
+      <c r="AD22" s="55"/>
+      <c r="AE22" s="55"/>
+      <c r="AF22" s="55"/>
+      <c r="AG22" s="55"/>
+      <c r="AH22" s="55"/>
+      <c r="AI22" s="55"/>
+      <c r="AJ22" s="55"/>
+      <c r="AK22" s="55"/>
+      <c r="AL22" s="55"/>
+      <c r="AM22" s="55"/>
+      <c r="AN22" s="55"/>
+      <c r="AO22" s="55"/>
+      <c r="AP22" s="55"/>
+      <c r="AQ22" s="55"/>
+      <c r="AR22" s="55"/>
+      <c r="AS22" s="55"/>
+      <c r="AT22" s="55"/>
+      <c r="AU22" s="55"/>
+      <c r="AV22" s="55"/>
+      <c r="AW22" s="55"/>
+      <c r="AX22" s="55"/>
+      <c r="AY22" s="55"/>
+      <c r="AZ22" s="55"/>
+      <c r="BA22" s="55"/>
+      <c r="BB22" s="55"/>
+      <c r="BC22" s="55"/>
+      <c r="BD22" s="55"/>
+      <c r="BE22" s="55"/>
+      <c r="BF22" s="55"/>
+      <c r="BG22" s="55"/>
+      <c r="BH22" s="55"/>
+      <c r="BI22" s="55"/>
+      <c r="BJ22" s="55"/>
+      <c r="BK22" s="55"/>
+      <c r="BL22" s="55"/>
+      <c r="BM22" s="55"/>
+      <c r="BN22" s="55"/>
+      <c r="BO22" s="55"/>
+      <c r="BP22" s="55"/>
+      <c r="BQ22" s="55"/>
+      <c r="BR22" s="55"/>
+      <c r="BS22" s="55"/>
+      <c r="BT22" s="55"/>
+      <c r="BU22" s="55"/>
+      <c r="BV22" s="55"/>
+      <c r="BW22" s="55"/>
+      <c r="BX22" s="55"/>
+      <c r="BY22" s="55"/>
+      <c r="BZ22" s="55"/>
+      <c r="CA22" s="55"/>
+      <c r="CB22" s="55"/>
+      <c r="CC22" s="55"/>
+      <c r="CD22" s="55"/>
+      <c r="CE22" s="55"/>
+      <c r="CF22" s="55"/>
+      <c r="CG22" s="55"/>
+      <c r="CH22" s="55"/>
+      <c r="CI22" s="55"/>
+      <c r="CJ22" s="55"/>
+      <c r="CK22" s="55"/>
+      <c r="CL22" s="55"/>
+      <c r="CM22" s="55"/>
+      <c r="CN22" s="55"/>
+      <c r="CO22" s="55"/>
+      <c r="CP22" s="55"/>
+      <c r="CQ22" s="55"/>
+      <c r="CR22" s="55"/>
+      <c r="CS22" s="55"/>
+      <c r="CT22" s="55"/>
+      <c r="CU22" s="55"/>
+      <c r="CV22" s="55"/>
+      <c r="CW22" s="55"/>
+      <c r="CX22" s="55"/>
+      <c r="CY22" s="55"/>
+      <c r="CZ22" s="55"/>
+      <c r="DA22" s="55"/>
+      <c r="DB22" s="55"/>
+      <c r="DC22" s="55"/>
+      <c r="DD22" s="55"/>
+      <c r="DE22" s="55"/>
+      <c r="DF22" s="55"/>
+      <c r="DG22" s="55"/>
+      <c r="DH22" s="55"/>
+      <c r="DI22" s="55"/>
+      <c r="DJ22" s="55"/>
+      <c r="DK22" s="55"/>
+      <c r="DL22" s="55"/>
+      <c r="DM22" s="55"/>
+    </row>
+    <row r="23" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
         <v>56</v>
       </c>
@@ -2514,117 +2598,117 @@
       <c r="H23" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="59"/>
-      <c r="T23" s="59"/>
-      <c r="U23" s="59"/>
-      <c r="V23" s="59"/>
-      <c r="W23" s="59"/>
-      <c r="X23" s="59"/>
-      <c r="Y23" s="59"/>
-      <c r="Z23" s="59"/>
-      <c r="AA23" s="59"/>
-      <c r="AB23" s="59"/>
-      <c r="AC23" s="59"/>
-      <c r="AD23" s="59"/>
-      <c r="AE23" s="59"/>
-      <c r="AF23" s="59"/>
-      <c r="AG23" s="59"/>
-      <c r="AH23" s="59"/>
-      <c r="AI23" s="59"/>
-      <c r="AJ23" s="59"/>
-      <c r="AK23" s="59"/>
-      <c r="AL23" s="59"/>
-      <c r="AM23" s="59"/>
-      <c r="AN23" s="59"/>
-      <c r="AO23" s="59"/>
-      <c r="AP23" s="59"/>
-      <c r="AQ23" s="59"/>
-      <c r="AR23" s="59"/>
-      <c r="AS23" s="59"/>
-      <c r="AT23" s="59"/>
-      <c r="AU23" s="59"/>
-      <c r="AV23" s="59"/>
-      <c r="AW23" s="59"/>
-      <c r="AX23" s="59"/>
-      <c r="AY23" s="59"/>
-      <c r="AZ23" s="59"/>
-      <c r="BA23" s="59"/>
-      <c r="BB23" s="59"/>
-      <c r="BC23" s="59"/>
-      <c r="BD23" s="59"/>
-      <c r="BE23" s="59"/>
-      <c r="BF23" s="59"/>
-      <c r="BG23" s="59"/>
-      <c r="BH23" s="59"/>
-      <c r="BI23" s="59"/>
-      <c r="BJ23" s="59"/>
-      <c r="BK23" s="59"/>
-      <c r="BL23" s="59"/>
-      <c r="BM23" s="59"/>
-      <c r="BN23" s="59"/>
-      <c r="BO23" s="59"/>
-      <c r="BP23" s="59"/>
-      <c r="BQ23" s="59"/>
-      <c r="BR23" s="59"/>
-      <c r="BS23" s="59"/>
-      <c r="BT23" s="59"/>
-      <c r="BU23" s="59"/>
-      <c r="BV23" s="59"/>
-      <c r="BW23" s="59"/>
-      <c r="BX23" s="59"/>
-      <c r="BY23" s="59"/>
-      <c r="BZ23" s="59"/>
-      <c r="CA23" s="59"/>
-      <c r="CB23" s="59"/>
-      <c r="CC23" s="59"/>
-      <c r="CD23" s="59"/>
-      <c r="CE23" s="59"/>
-      <c r="CF23" s="59"/>
-      <c r="CG23" s="59"/>
-      <c r="CH23" s="59"/>
-      <c r="CI23" s="59"/>
-      <c r="CJ23" s="59"/>
-      <c r="CK23" s="59"/>
-      <c r="CL23" s="59"/>
-      <c r="CM23" s="59"/>
-      <c r="CN23" s="59"/>
-      <c r="CO23" s="59"/>
-      <c r="CP23" s="59"/>
-      <c r="CQ23" s="59"/>
-      <c r="CR23" s="59"/>
-      <c r="CS23" s="59"/>
-      <c r="CT23" s="59"/>
-      <c r="CU23" s="59"/>
-      <c r="CV23" s="59"/>
-      <c r="CW23" s="59"/>
-      <c r="CX23" s="59"/>
-      <c r="CY23" s="59"/>
-      <c r="CZ23" s="59"/>
-      <c r="DA23" s="59"/>
-      <c r="DB23" s="59"/>
-      <c r="DC23" s="59"/>
-      <c r="DD23" s="59"/>
-      <c r="DE23" s="59"/>
-      <c r="DF23" s="59"/>
-      <c r="DG23" s="59"/>
-      <c r="DH23" s="59"/>
-      <c r="DI23" s="59"/>
-      <c r="DJ23" s="59"/>
-      <c r="DK23" s="59"/>
-      <c r="DL23" s="59"/>
-      <c r="DM23" s="59"/>
-    </row>
-    <row r="24" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="55"/>
+      <c r="J23" s="55"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="55"/>
+      <c r="Z23" s="55"/>
+      <c r="AA23" s="55"/>
+      <c r="AB23" s="55"/>
+      <c r="AC23" s="55"/>
+      <c r="AD23" s="55"/>
+      <c r="AE23" s="55"/>
+      <c r="AF23" s="55"/>
+      <c r="AG23" s="55"/>
+      <c r="AH23" s="55"/>
+      <c r="AI23" s="55"/>
+      <c r="AJ23" s="55"/>
+      <c r="AK23" s="55"/>
+      <c r="AL23" s="55"/>
+      <c r="AM23" s="55"/>
+      <c r="AN23" s="55"/>
+      <c r="AO23" s="55"/>
+      <c r="AP23" s="55"/>
+      <c r="AQ23" s="55"/>
+      <c r="AR23" s="55"/>
+      <c r="AS23" s="55"/>
+      <c r="AT23" s="55"/>
+      <c r="AU23" s="55"/>
+      <c r="AV23" s="55"/>
+      <c r="AW23" s="55"/>
+      <c r="AX23" s="55"/>
+      <c r="AY23" s="55"/>
+      <c r="AZ23" s="55"/>
+      <c r="BA23" s="55"/>
+      <c r="BB23" s="55"/>
+      <c r="BC23" s="55"/>
+      <c r="BD23" s="55"/>
+      <c r="BE23" s="55"/>
+      <c r="BF23" s="55"/>
+      <c r="BG23" s="55"/>
+      <c r="BH23" s="55"/>
+      <c r="BI23" s="55"/>
+      <c r="BJ23" s="55"/>
+      <c r="BK23" s="55"/>
+      <c r="BL23" s="55"/>
+      <c r="BM23" s="55"/>
+      <c r="BN23" s="55"/>
+      <c r="BO23" s="55"/>
+      <c r="BP23" s="55"/>
+      <c r="BQ23" s="55"/>
+      <c r="BR23" s="55"/>
+      <c r="BS23" s="55"/>
+      <c r="BT23" s="55"/>
+      <c r="BU23" s="55"/>
+      <c r="BV23" s="55"/>
+      <c r="BW23" s="55"/>
+      <c r="BX23" s="55"/>
+      <c r="BY23" s="55"/>
+      <c r="BZ23" s="55"/>
+      <c r="CA23" s="55"/>
+      <c r="CB23" s="55"/>
+      <c r="CC23" s="55"/>
+      <c r="CD23" s="55"/>
+      <c r="CE23" s="55"/>
+      <c r="CF23" s="55"/>
+      <c r="CG23" s="55"/>
+      <c r="CH23" s="55"/>
+      <c r="CI23" s="55"/>
+      <c r="CJ23" s="55"/>
+      <c r="CK23" s="55"/>
+      <c r="CL23" s="55"/>
+      <c r="CM23" s="55"/>
+      <c r="CN23" s="55"/>
+      <c r="CO23" s="55"/>
+      <c r="CP23" s="55"/>
+      <c r="CQ23" s="55"/>
+      <c r="CR23" s="55"/>
+      <c r="CS23" s="55"/>
+      <c r="CT23" s="55"/>
+      <c r="CU23" s="55"/>
+      <c r="CV23" s="55"/>
+      <c r="CW23" s="55"/>
+      <c r="CX23" s="55"/>
+      <c r="CY23" s="55"/>
+      <c r="CZ23" s="55"/>
+      <c r="DA23" s="55"/>
+      <c r="DB23" s="55"/>
+      <c r="DC23" s="55"/>
+      <c r="DD23" s="55"/>
+      <c r="DE23" s="55"/>
+      <c r="DF23" s="55"/>
+      <c r="DG23" s="55"/>
+      <c r="DH23" s="55"/>
+      <c r="DI23" s="55"/>
+      <c r="DJ23" s="55"/>
+      <c r="DK23" s="55"/>
+      <c r="DL23" s="55"/>
+      <c r="DM23" s="55"/>
+    </row>
+    <row r="24" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="31" t="s">
         <v>33</v>
       </c>
@@ -2640,7 +2724,7 @@
       <c r="E24" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="52">
+      <c r="F24" s="48">
         <v>13</v>
       </c>
       <c r="G24" s="7">
@@ -2649,117 +2733,117 @@
       <c r="H24" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="59"/>
-      <c r="T24" s="59"/>
-      <c r="U24" s="59"/>
-      <c r="V24" s="59"/>
-      <c r="W24" s="59"/>
-      <c r="X24" s="59"/>
-      <c r="Y24" s="59"/>
-      <c r="Z24" s="59"/>
-      <c r="AA24" s="59"/>
-      <c r="AB24" s="59"/>
-      <c r="AC24" s="59"/>
-      <c r="AD24" s="59"/>
-      <c r="AE24" s="59"/>
-      <c r="AF24" s="59"/>
-      <c r="AG24" s="59"/>
-      <c r="AH24" s="59"/>
-      <c r="AI24" s="59"/>
-      <c r="AJ24" s="59"/>
-      <c r="AK24" s="59"/>
-      <c r="AL24" s="59"/>
-      <c r="AM24" s="59"/>
-      <c r="AN24" s="59"/>
-      <c r="AO24" s="59"/>
-      <c r="AP24" s="59"/>
-      <c r="AQ24" s="59"/>
-      <c r="AR24" s="59"/>
-      <c r="AS24" s="59"/>
-      <c r="AT24" s="59"/>
-      <c r="AU24" s="59"/>
-      <c r="AV24" s="59"/>
-      <c r="AW24" s="59"/>
-      <c r="AX24" s="59"/>
-      <c r="AY24" s="59"/>
-      <c r="AZ24" s="59"/>
-      <c r="BA24" s="59"/>
-      <c r="BB24" s="59"/>
-      <c r="BC24" s="59"/>
-      <c r="BD24" s="59"/>
-      <c r="BE24" s="59"/>
-      <c r="BF24" s="59"/>
-      <c r="BG24" s="59"/>
-      <c r="BH24" s="59"/>
-      <c r="BI24" s="59"/>
-      <c r="BJ24" s="59"/>
-      <c r="BK24" s="59"/>
-      <c r="BL24" s="59"/>
-      <c r="BM24" s="59"/>
-      <c r="BN24" s="59"/>
-      <c r="BO24" s="59"/>
-      <c r="BP24" s="59"/>
-      <c r="BQ24" s="59"/>
-      <c r="BR24" s="59"/>
-      <c r="BS24" s="59"/>
-      <c r="BT24" s="59"/>
-      <c r="BU24" s="59"/>
-      <c r="BV24" s="59"/>
-      <c r="BW24" s="59"/>
-      <c r="BX24" s="59"/>
-      <c r="BY24" s="59"/>
-      <c r="BZ24" s="59"/>
-      <c r="CA24" s="59"/>
-      <c r="CB24" s="59"/>
-      <c r="CC24" s="59"/>
-      <c r="CD24" s="59"/>
-      <c r="CE24" s="59"/>
-      <c r="CF24" s="59"/>
-      <c r="CG24" s="59"/>
-      <c r="CH24" s="59"/>
-      <c r="CI24" s="59"/>
-      <c r="CJ24" s="59"/>
-      <c r="CK24" s="59"/>
-      <c r="CL24" s="59"/>
-      <c r="CM24" s="59"/>
-      <c r="CN24" s="59"/>
-      <c r="CO24" s="59"/>
-      <c r="CP24" s="59"/>
-      <c r="CQ24" s="59"/>
-      <c r="CR24" s="59"/>
-      <c r="CS24" s="59"/>
-      <c r="CT24" s="59"/>
-      <c r="CU24" s="59"/>
-      <c r="CV24" s="59"/>
-      <c r="CW24" s="59"/>
-      <c r="CX24" s="59"/>
-      <c r="CY24" s="59"/>
-      <c r="CZ24" s="59"/>
-      <c r="DA24" s="59"/>
-      <c r="DB24" s="59"/>
-      <c r="DC24" s="59"/>
-      <c r="DD24" s="59"/>
-      <c r="DE24" s="59"/>
-      <c r="DF24" s="59"/>
-      <c r="DG24" s="59"/>
-      <c r="DH24" s="59"/>
-      <c r="DI24" s="59"/>
-      <c r="DJ24" s="59"/>
-      <c r="DK24" s="59"/>
-      <c r="DL24" s="59"/>
-      <c r="DM24" s="59"/>
-    </row>
-    <row r="25" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="55"/>
+      <c r="T24" s="55"/>
+      <c r="U24" s="55"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="55"/>
+      <c r="Z24" s="55"/>
+      <c r="AA24" s="55"/>
+      <c r="AB24" s="55"/>
+      <c r="AC24" s="55"/>
+      <c r="AD24" s="55"/>
+      <c r="AE24" s="55"/>
+      <c r="AF24" s="55"/>
+      <c r="AG24" s="55"/>
+      <c r="AH24" s="55"/>
+      <c r="AI24" s="55"/>
+      <c r="AJ24" s="55"/>
+      <c r="AK24" s="55"/>
+      <c r="AL24" s="55"/>
+      <c r="AM24" s="55"/>
+      <c r="AN24" s="55"/>
+      <c r="AO24" s="55"/>
+      <c r="AP24" s="55"/>
+      <c r="AQ24" s="55"/>
+      <c r="AR24" s="55"/>
+      <c r="AS24" s="55"/>
+      <c r="AT24" s="55"/>
+      <c r="AU24" s="55"/>
+      <c r="AV24" s="55"/>
+      <c r="AW24" s="55"/>
+      <c r="AX24" s="55"/>
+      <c r="AY24" s="55"/>
+      <c r="AZ24" s="55"/>
+      <c r="BA24" s="55"/>
+      <c r="BB24" s="55"/>
+      <c r="BC24" s="55"/>
+      <c r="BD24" s="55"/>
+      <c r="BE24" s="55"/>
+      <c r="BF24" s="55"/>
+      <c r="BG24" s="55"/>
+      <c r="BH24" s="55"/>
+      <c r="BI24" s="55"/>
+      <c r="BJ24" s="55"/>
+      <c r="BK24" s="55"/>
+      <c r="BL24" s="55"/>
+      <c r="BM24" s="55"/>
+      <c r="BN24" s="55"/>
+      <c r="BO24" s="55"/>
+      <c r="BP24" s="55"/>
+      <c r="BQ24" s="55"/>
+      <c r="BR24" s="55"/>
+      <c r="BS24" s="55"/>
+      <c r="BT24" s="55"/>
+      <c r="BU24" s="55"/>
+      <c r="BV24" s="55"/>
+      <c r="BW24" s="55"/>
+      <c r="BX24" s="55"/>
+      <c r="BY24" s="55"/>
+      <c r="BZ24" s="55"/>
+      <c r="CA24" s="55"/>
+      <c r="CB24" s="55"/>
+      <c r="CC24" s="55"/>
+      <c r="CD24" s="55"/>
+      <c r="CE24" s="55"/>
+      <c r="CF24" s="55"/>
+      <c r="CG24" s="55"/>
+      <c r="CH24" s="55"/>
+      <c r="CI24" s="55"/>
+      <c r="CJ24" s="55"/>
+      <c r="CK24" s="55"/>
+      <c r="CL24" s="55"/>
+      <c r="CM24" s="55"/>
+      <c r="CN24" s="55"/>
+      <c r="CO24" s="55"/>
+      <c r="CP24" s="55"/>
+      <c r="CQ24" s="55"/>
+      <c r="CR24" s="55"/>
+      <c r="CS24" s="55"/>
+      <c r="CT24" s="55"/>
+      <c r="CU24" s="55"/>
+      <c r="CV24" s="55"/>
+      <c r="CW24" s="55"/>
+      <c r="CX24" s="55"/>
+      <c r="CY24" s="55"/>
+      <c r="CZ24" s="55"/>
+      <c r="DA24" s="55"/>
+      <c r="DB24" s="55"/>
+      <c r="DC24" s="55"/>
+      <c r="DD24" s="55"/>
+      <c r="DE24" s="55"/>
+      <c r="DF24" s="55"/>
+      <c r="DG24" s="55"/>
+      <c r="DH24" s="55"/>
+      <c r="DI24" s="55"/>
+      <c r="DJ24" s="55"/>
+      <c r="DK24" s="55"/>
+      <c r="DL24" s="55"/>
+      <c r="DM24" s="55"/>
+    </row>
+    <row r="25" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="31" t="s">
         <v>48</v>
       </c>
@@ -2775,124 +2859,124 @@
       <c r="E25" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="65">
+      <c r="F25" s="61">
         <v>21</v>
       </c>
-      <c r="G25" s="77"/>
-      <c r="H25" s="82" t="s">
+      <c r="G25" s="67"/>
+      <c r="H25" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="59"/>
-      <c r="T25" s="59"/>
-      <c r="U25" s="59"/>
-      <c r="V25" s="59"/>
-      <c r="W25" s="59"/>
-      <c r="X25" s="59"/>
-      <c r="Y25" s="59"/>
-      <c r="Z25" s="59"/>
-      <c r="AA25" s="59"/>
-      <c r="AB25" s="59"/>
-      <c r="AC25" s="59"/>
-      <c r="AD25" s="59"/>
-      <c r="AE25" s="59"/>
-      <c r="AF25" s="59"/>
-      <c r="AG25" s="59"/>
-      <c r="AH25" s="59"/>
-      <c r="AI25" s="59"/>
-      <c r="AJ25" s="59"/>
-      <c r="AK25" s="59"/>
-      <c r="AL25" s="59"/>
-      <c r="AM25" s="59"/>
-      <c r="AN25" s="59"/>
-      <c r="AO25" s="59"/>
-      <c r="AP25" s="59"/>
-      <c r="AQ25" s="59"/>
-      <c r="AR25" s="59"/>
-      <c r="AS25" s="59"/>
-      <c r="AT25" s="59"/>
-      <c r="AU25" s="59"/>
-      <c r="AV25" s="59"/>
-      <c r="AW25" s="59"/>
-      <c r="AX25" s="59"/>
-      <c r="AY25" s="59"/>
-      <c r="AZ25" s="59"/>
-      <c r="BA25" s="59"/>
-      <c r="BB25" s="59"/>
-      <c r="BC25" s="59"/>
-      <c r="BD25" s="59"/>
-      <c r="BE25" s="59"/>
-      <c r="BF25" s="59"/>
-      <c r="BG25" s="59"/>
-      <c r="BH25" s="59"/>
-      <c r="BI25" s="59"/>
-      <c r="BJ25" s="59"/>
-      <c r="BK25" s="59"/>
-      <c r="BL25" s="59"/>
-      <c r="BM25" s="59"/>
-      <c r="BN25" s="59"/>
-      <c r="BO25" s="59"/>
-      <c r="BP25" s="59"/>
-      <c r="BQ25" s="59"/>
-      <c r="BR25" s="59"/>
-      <c r="BS25" s="59"/>
-      <c r="BT25" s="59"/>
-      <c r="BU25" s="59"/>
-      <c r="BV25" s="59"/>
-      <c r="BW25" s="59"/>
-      <c r="BX25" s="59"/>
-      <c r="BY25" s="59"/>
-      <c r="BZ25" s="59"/>
-      <c r="CA25" s="59"/>
-      <c r="CB25" s="59"/>
-      <c r="CC25" s="59"/>
-      <c r="CD25" s="59"/>
-      <c r="CE25" s="59"/>
-      <c r="CF25" s="59"/>
-      <c r="CG25" s="59"/>
-      <c r="CH25" s="59"/>
-      <c r="CI25" s="59"/>
-      <c r="CJ25" s="59"/>
-      <c r="CK25" s="59"/>
-      <c r="CL25" s="59"/>
-      <c r="CM25" s="59"/>
-      <c r="CN25" s="59"/>
-      <c r="CO25" s="59"/>
-      <c r="CP25" s="59"/>
-      <c r="CQ25" s="59"/>
-      <c r="CR25" s="59"/>
-      <c r="CS25" s="59"/>
-      <c r="CT25" s="59"/>
-      <c r="CU25" s="59"/>
-      <c r="CV25" s="59"/>
-      <c r="CW25" s="59"/>
-      <c r="CX25" s="59"/>
-      <c r="CY25" s="59"/>
-      <c r="CZ25" s="59"/>
-      <c r="DA25" s="59"/>
-      <c r="DB25" s="59"/>
-      <c r="DC25" s="59"/>
-      <c r="DD25" s="59"/>
-      <c r="DE25" s="59"/>
-      <c r="DF25" s="59"/>
-      <c r="DG25" s="59"/>
-      <c r="DH25" s="59"/>
-      <c r="DI25" s="59"/>
-      <c r="DJ25" s="59"/>
-      <c r="DK25" s="59"/>
-      <c r="DL25" s="59"/>
-      <c r="DM25" s="59"/>
-    </row>
-    <row r="26" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="55"/>
+      <c r="T25" s="55"/>
+      <c r="U25" s="55"/>
+      <c r="V25" s="55"/>
+      <c r="W25" s="55"/>
+      <c r="X25" s="55"/>
+      <c r="Y25" s="55"/>
+      <c r="Z25" s="55"/>
+      <c r="AA25" s="55"/>
+      <c r="AB25" s="55"/>
+      <c r="AC25" s="55"/>
+      <c r="AD25" s="55"/>
+      <c r="AE25" s="55"/>
+      <c r="AF25" s="55"/>
+      <c r="AG25" s="55"/>
+      <c r="AH25" s="55"/>
+      <c r="AI25" s="55"/>
+      <c r="AJ25" s="55"/>
+      <c r="AK25" s="55"/>
+      <c r="AL25" s="55"/>
+      <c r="AM25" s="55"/>
+      <c r="AN25" s="55"/>
+      <c r="AO25" s="55"/>
+      <c r="AP25" s="55"/>
+      <c r="AQ25" s="55"/>
+      <c r="AR25" s="55"/>
+      <c r="AS25" s="55"/>
+      <c r="AT25" s="55"/>
+      <c r="AU25" s="55"/>
+      <c r="AV25" s="55"/>
+      <c r="AW25" s="55"/>
+      <c r="AX25" s="55"/>
+      <c r="AY25" s="55"/>
+      <c r="AZ25" s="55"/>
+      <c r="BA25" s="55"/>
+      <c r="BB25" s="55"/>
+      <c r="BC25" s="55"/>
+      <c r="BD25" s="55"/>
+      <c r="BE25" s="55"/>
+      <c r="BF25" s="55"/>
+      <c r="BG25" s="55"/>
+      <c r="BH25" s="55"/>
+      <c r="BI25" s="55"/>
+      <c r="BJ25" s="55"/>
+      <c r="BK25" s="55"/>
+      <c r="BL25" s="55"/>
+      <c r="BM25" s="55"/>
+      <c r="BN25" s="55"/>
+      <c r="BO25" s="55"/>
+      <c r="BP25" s="55"/>
+      <c r="BQ25" s="55"/>
+      <c r="BR25" s="55"/>
+      <c r="BS25" s="55"/>
+      <c r="BT25" s="55"/>
+      <c r="BU25" s="55"/>
+      <c r="BV25" s="55"/>
+      <c r="BW25" s="55"/>
+      <c r="BX25" s="55"/>
+      <c r="BY25" s="55"/>
+      <c r="BZ25" s="55"/>
+      <c r="CA25" s="55"/>
+      <c r="CB25" s="55"/>
+      <c r="CC25" s="55"/>
+      <c r="CD25" s="55"/>
+      <c r="CE25" s="55"/>
+      <c r="CF25" s="55"/>
+      <c r="CG25" s="55"/>
+      <c r="CH25" s="55"/>
+      <c r="CI25" s="55"/>
+      <c r="CJ25" s="55"/>
+      <c r="CK25" s="55"/>
+      <c r="CL25" s="55"/>
+      <c r="CM25" s="55"/>
+      <c r="CN25" s="55"/>
+      <c r="CO25" s="55"/>
+      <c r="CP25" s="55"/>
+      <c r="CQ25" s="55"/>
+      <c r="CR25" s="55"/>
+      <c r="CS25" s="55"/>
+      <c r="CT25" s="55"/>
+      <c r="CU25" s="55"/>
+      <c r="CV25" s="55"/>
+      <c r="CW25" s="55"/>
+      <c r="CX25" s="55"/>
+      <c r="CY25" s="55"/>
+      <c r="CZ25" s="55"/>
+      <c r="DA25" s="55"/>
+      <c r="DB25" s="55"/>
+      <c r="DC25" s="55"/>
+      <c r="DD25" s="55"/>
+      <c r="DE25" s="55"/>
+      <c r="DF25" s="55"/>
+      <c r="DG25" s="55"/>
+      <c r="DH25" s="55"/>
+      <c r="DI25" s="55"/>
+      <c r="DJ25" s="55"/>
+      <c r="DK25" s="55"/>
+      <c r="DL25" s="55"/>
+      <c r="DM25" s="55"/>
+    </row>
+    <row r="26" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>49</v>
       </c>
@@ -2905,127 +2989,127 @@
       <c r="D26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="76">
+      <c r="F26" s="66">
         <v>5</v>
       </c>
-      <c r="G26" s="77"/>
-      <c r="H26" s="82" t="s">
+      <c r="G26" s="67"/>
+      <c r="H26" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="59"/>
-      <c r="T26" s="59"/>
-      <c r="U26" s="59"/>
-      <c r="V26" s="59"/>
-      <c r="W26" s="59"/>
-      <c r="X26" s="59"/>
-      <c r="Y26" s="59"/>
-      <c r="Z26" s="59"/>
-      <c r="AA26" s="59"/>
-      <c r="AB26" s="59"/>
-      <c r="AC26" s="59"/>
-      <c r="AD26" s="59"/>
-      <c r="AE26" s="59"/>
-      <c r="AF26" s="59"/>
-      <c r="AG26" s="59"/>
-      <c r="AH26" s="59"/>
-      <c r="AI26" s="59"/>
-      <c r="AJ26" s="59"/>
-      <c r="AK26" s="59"/>
-      <c r="AL26" s="59"/>
-      <c r="AM26" s="59"/>
-      <c r="AN26" s="59"/>
-      <c r="AO26" s="59"/>
-      <c r="AP26" s="59"/>
-      <c r="AQ26" s="59"/>
-      <c r="AR26" s="59"/>
-      <c r="AS26" s="59"/>
-      <c r="AT26" s="59"/>
-      <c r="AU26" s="59"/>
-      <c r="AV26" s="59"/>
-      <c r="AW26" s="59"/>
-      <c r="AX26" s="59"/>
-      <c r="AY26" s="59"/>
-      <c r="AZ26" s="59"/>
-      <c r="BA26" s="59"/>
-      <c r="BB26" s="59"/>
-      <c r="BC26" s="59"/>
-      <c r="BD26" s="59"/>
-      <c r="BE26" s="59"/>
-      <c r="BF26" s="59"/>
-      <c r="BG26" s="59"/>
-      <c r="BH26" s="59"/>
-      <c r="BI26" s="59"/>
-      <c r="BJ26" s="59"/>
-      <c r="BK26" s="59"/>
-      <c r="BL26" s="59"/>
-      <c r="BM26" s="59"/>
-      <c r="BN26" s="59"/>
-      <c r="BO26" s="59"/>
-      <c r="BP26" s="59"/>
-      <c r="BQ26" s="59"/>
-      <c r="BR26" s="59"/>
-      <c r="BS26" s="59"/>
-      <c r="BT26" s="59"/>
-      <c r="BU26" s="59"/>
-      <c r="BV26" s="59"/>
-      <c r="BW26" s="59"/>
-      <c r="BX26" s="59"/>
-      <c r="BY26" s="59"/>
-      <c r="BZ26" s="59"/>
-      <c r="CA26" s="59"/>
-      <c r="CB26" s="59"/>
-      <c r="CC26" s="59"/>
-      <c r="CD26" s="59"/>
-      <c r="CE26" s="59"/>
-      <c r="CF26" s="59"/>
-      <c r="CG26" s="59"/>
-      <c r="CH26" s="59"/>
-      <c r="CI26" s="59"/>
-      <c r="CJ26" s="59"/>
-      <c r="CK26" s="59"/>
-      <c r="CL26" s="59"/>
-      <c r="CM26" s="59"/>
-      <c r="CN26" s="59"/>
-      <c r="CO26" s="59"/>
-      <c r="CP26" s="59"/>
-      <c r="CQ26" s="59"/>
-      <c r="CR26" s="59"/>
-      <c r="CS26" s="59"/>
-      <c r="CT26" s="59"/>
-      <c r="CU26" s="59"/>
-      <c r="CV26" s="59"/>
-      <c r="CW26" s="59"/>
-      <c r="CX26" s="59"/>
-      <c r="CY26" s="59"/>
-      <c r="CZ26" s="59"/>
-      <c r="DA26" s="59"/>
-      <c r="DB26" s="59"/>
-      <c r="DC26" s="59"/>
-      <c r="DD26" s="59"/>
-      <c r="DE26" s="59"/>
-      <c r="DF26" s="59"/>
-      <c r="DG26" s="59"/>
-      <c r="DH26" s="59"/>
-      <c r="DI26" s="59"/>
-      <c r="DJ26" s="59"/>
-      <c r="DK26" s="59"/>
-      <c r="DL26" s="59"/>
-      <c r="DM26" s="59"/>
-    </row>
-    <row r="27" spans="1:117" s="42" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
+      <c r="V26" s="55"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="55"/>
+      <c r="Y26" s="55"/>
+      <c r="Z26" s="55"/>
+      <c r="AA26" s="55"/>
+      <c r="AB26" s="55"/>
+      <c r="AC26" s="55"/>
+      <c r="AD26" s="55"/>
+      <c r="AE26" s="55"/>
+      <c r="AF26" s="55"/>
+      <c r="AG26" s="55"/>
+      <c r="AH26" s="55"/>
+      <c r="AI26" s="55"/>
+      <c r="AJ26" s="55"/>
+      <c r="AK26" s="55"/>
+      <c r="AL26" s="55"/>
+      <c r="AM26" s="55"/>
+      <c r="AN26" s="55"/>
+      <c r="AO26" s="55"/>
+      <c r="AP26" s="55"/>
+      <c r="AQ26" s="55"/>
+      <c r="AR26" s="55"/>
+      <c r="AS26" s="55"/>
+      <c r="AT26" s="55"/>
+      <c r="AU26" s="55"/>
+      <c r="AV26" s="55"/>
+      <c r="AW26" s="55"/>
+      <c r="AX26" s="55"/>
+      <c r="AY26" s="55"/>
+      <c r="AZ26" s="55"/>
+      <c r="BA26" s="55"/>
+      <c r="BB26" s="55"/>
+      <c r="BC26" s="55"/>
+      <c r="BD26" s="55"/>
+      <c r="BE26" s="55"/>
+      <c r="BF26" s="55"/>
+      <c r="BG26" s="55"/>
+      <c r="BH26" s="55"/>
+      <c r="BI26" s="55"/>
+      <c r="BJ26" s="55"/>
+      <c r="BK26" s="55"/>
+      <c r="BL26" s="55"/>
+      <c r="BM26" s="55"/>
+      <c r="BN26" s="55"/>
+      <c r="BO26" s="55"/>
+      <c r="BP26" s="55"/>
+      <c r="BQ26" s="55"/>
+      <c r="BR26" s="55"/>
+      <c r="BS26" s="55"/>
+      <c r="BT26" s="55"/>
+      <c r="BU26" s="55"/>
+      <c r="BV26" s="55"/>
+      <c r="BW26" s="55"/>
+      <c r="BX26" s="55"/>
+      <c r="BY26" s="55"/>
+      <c r="BZ26" s="55"/>
+      <c r="CA26" s="55"/>
+      <c r="CB26" s="55"/>
+      <c r="CC26" s="55"/>
+      <c r="CD26" s="55"/>
+      <c r="CE26" s="55"/>
+      <c r="CF26" s="55"/>
+      <c r="CG26" s="55"/>
+      <c r="CH26" s="55"/>
+      <c r="CI26" s="55"/>
+      <c r="CJ26" s="55"/>
+      <c r="CK26" s="55"/>
+      <c r="CL26" s="55"/>
+      <c r="CM26" s="55"/>
+      <c r="CN26" s="55"/>
+      <c r="CO26" s="55"/>
+      <c r="CP26" s="55"/>
+      <c r="CQ26" s="55"/>
+      <c r="CR26" s="55"/>
+      <c r="CS26" s="55"/>
+      <c r="CT26" s="55"/>
+      <c r="CU26" s="55"/>
+      <c r="CV26" s="55"/>
+      <c r="CW26" s="55"/>
+      <c r="CX26" s="55"/>
+      <c r="CY26" s="55"/>
+      <c r="CZ26" s="55"/>
+      <c r="DA26" s="55"/>
+      <c r="DB26" s="55"/>
+      <c r="DC26" s="55"/>
+      <c r="DD26" s="55"/>
+      <c r="DE26" s="55"/>
+      <c r="DF26" s="55"/>
+      <c r="DG26" s="55"/>
+      <c r="DH26" s="55"/>
+      <c r="DI26" s="55"/>
+      <c r="DJ26" s="55"/>
+      <c r="DK26" s="55"/>
+      <c r="DL26" s="55"/>
+      <c r="DM26" s="55"/>
+    </row>
+    <row r="27" spans="1:117" s="38" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="31" t="s">
         <v>51</v>
       </c>
@@ -3041,124 +3125,124 @@
       <c r="E27" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="75">
+      <c r="F27" s="65">
         <v>13</v>
       </c>
-      <c r="G27" s="77"/>
-      <c r="H27" s="82" t="s">
+      <c r="G27" s="67"/>
+      <c r="H27" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="59"/>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="59"/>
-      <c r="W27" s="59"/>
-      <c r="X27" s="59"/>
-      <c r="Y27" s="59"/>
-      <c r="Z27" s="59"/>
-      <c r="AA27" s="59"/>
-      <c r="AB27" s="59"/>
-      <c r="AC27" s="59"/>
-      <c r="AD27" s="59"/>
-      <c r="AE27" s="59"/>
-      <c r="AF27" s="59"/>
-      <c r="AG27" s="59"/>
-      <c r="AH27" s="59"/>
-      <c r="AI27" s="59"/>
-      <c r="AJ27" s="59"/>
-      <c r="AK27" s="59"/>
-      <c r="AL27" s="59"/>
-      <c r="AM27" s="59"/>
-      <c r="AN27" s="59"/>
-      <c r="AO27" s="59"/>
-      <c r="AP27" s="59"/>
-      <c r="AQ27" s="59"/>
-      <c r="AR27" s="59"/>
-      <c r="AS27" s="59"/>
-      <c r="AT27" s="59"/>
-      <c r="AU27" s="59"/>
-      <c r="AV27" s="59"/>
-      <c r="AW27" s="59"/>
-      <c r="AX27" s="59"/>
-      <c r="AY27" s="59"/>
-      <c r="AZ27" s="59"/>
-      <c r="BA27" s="59"/>
-      <c r="BB27" s="59"/>
-      <c r="BC27" s="59"/>
-      <c r="BD27" s="59"/>
-      <c r="BE27" s="59"/>
-      <c r="BF27" s="59"/>
-      <c r="BG27" s="59"/>
-      <c r="BH27" s="59"/>
-      <c r="BI27" s="59"/>
-      <c r="BJ27" s="59"/>
-      <c r="BK27" s="59"/>
-      <c r="BL27" s="59"/>
-      <c r="BM27" s="59"/>
-      <c r="BN27" s="59"/>
-      <c r="BO27" s="59"/>
-      <c r="BP27" s="59"/>
-      <c r="BQ27" s="59"/>
-      <c r="BR27" s="59"/>
-      <c r="BS27" s="59"/>
-      <c r="BT27" s="59"/>
-      <c r="BU27" s="59"/>
-      <c r="BV27" s="59"/>
-      <c r="BW27" s="59"/>
-      <c r="BX27" s="59"/>
-      <c r="BY27" s="59"/>
-      <c r="BZ27" s="59"/>
-      <c r="CA27" s="59"/>
-      <c r="CB27" s="59"/>
-      <c r="CC27" s="59"/>
-      <c r="CD27" s="59"/>
-      <c r="CE27" s="59"/>
-      <c r="CF27" s="59"/>
-      <c r="CG27" s="59"/>
-      <c r="CH27" s="59"/>
-      <c r="CI27" s="59"/>
-      <c r="CJ27" s="59"/>
-      <c r="CK27" s="59"/>
-      <c r="CL27" s="59"/>
-      <c r="CM27" s="59"/>
-      <c r="CN27" s="59"/>
-      <c r="CO27" s="59"/>
-      <c r="CP27" s="59"/>
-      <c r="CQ27" s="59"/>
-      <c r="CR27" s="59"/>
-      <c r="CS27" s="59"/>
-      <c r="CT27" s="59"/>
-      <c r="CU27" s="59"/>
-      <c r="CV27" s="59"/>
-      <c r="CW27" s="59"/>
-      <c r="CX27" s="59"/>
-      <c r="CY27" s="59"/>
-      <c r="CZ27" s="59"/>
-      <c r="DA27" s="59"/>
-      <c r="DB27" s="59"/>
-      <c r="DC27" s="59"/>
-      <c r="DD27" s="59"/>
-      <c r="DE27" s="59"/>
-      <c r="DF27" s="59"/>
-      <c r="DG27" s="59"/>
-      <c r="DH27" s="59"/>
-      <c r="DI27" s="59"/>
-      <c r="DJ27" s="59"/>
-      <c r="DK27" s="59"/>
-      <c r="DL27" s="59"/>
-      <c r="DM27" s="59"/>
-    </row>
-    <row r="28" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="55"/>
+      <c r="J27" s="55"/>
+      <c r="K27" s="55"/>
+      <c r="L27" s="55"/>
+      <c r="M27" s="55"/>
+      <c r="N27" s="55"/>
+      <c r="O27" s="55"/>
+      <c r="P27" s="55"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="55"/>
+      <c r="T27" s="55"/>
+      <c r="U27" s="55"/>
+      <c r="V27" s="55"/>
+      <c r="W27" s="55"/>
+      <c r="X27" s="55"/>
+      <c r="Y27" s="55"/>
+      <c r="Z27" s="55"/>
+      <c r="AA27" s="55"/>
+      <c r="AB27" s="55"/>
+      <c r="AC27" s="55"/>
+      <c r="AD27" s="55"/>
+      <c r="AE27" s="55"/>
+      <c r="AF27" s="55"/>
+      <c r="AG27" s="55"/>
+      <c r="AH27" s="55"/>
+      <c r="AI27" s="55"/>
+      <c r="AJ27" s="55"/>
+      <c r="AK27" s="55"/>
+      <c r="AL27" s="55"/>
+      <c r="AM27" s="55"/>
+      <c r="AN27" s="55"/>
+      <c r="AO27" s="55"/>
+      <c r="AP27" s="55"/>
+      <c r="AQ27" s="55"/>
+      <c r="AR27" s="55"/>
+      <c r="AS27" s="55"/>
+      <c r="AT27" s="55"/>
+      <c r="AU27" s="55"/>
+      <c r="AV27" s="55"/>
+      <c r="AW27" s="55"/>
+      <c r="AX27" s="55"/>
+      <c r="AY27" s="55"/>
+      <c r="AZ27" s="55"/>
+      <c r="BA27" s="55"/>
+      <c r="BB27" s="55"/>
+      <c r="BC27" s="55"/>
+      <c r="BD27" s="55"/>
+      <c r="BE27" s="55"/>
+      <c r="BF27" s="55"/>
+      <c r="BG27" s="55"/>
+      <c r="BH27" s="55"/>
+      <c r="BI27" s="55"/>
+      <c r="BJ27" s="55"/>
+      <c r="BK27" s="55"/>
+      <c r="BL27" s="55"/>
+      <c r="BM27" s="55"/>
+      <c r="BN27" s="55"/>
+      <c r="BO27" s="55"/>
+      <c r="BP27" s="55"/>
+      <c r="BQ27" s="55"/>
+      <c r="BR27" s="55"/>
+      <c r="BS27" s="55"/>
+      <c r="BT27" s="55"/>
+      <c r="BU27" s="55"/>
+      <c r="BV27" s="55"/>
+      <c r="BW27" s="55"/>
+      <c r="BX27" s="55"/>
+      <c r="BY27" s="55"/>
+      <c r="BZ27" s="55"/>
+      <c r="CA27" s="55"/>
+      <c r="CB27" s="55"/>
+      <c r="CC27" s="55"/>
+      <c r="CD27" s="55"/>
+      <c r="CE27" s="55"/>
+      <c r="CF27" s="55"/>
+      <c r="CG27" s="55"/>
+      <c r="CH27" s="55"/>
+      <c r="CI27" s="55"/>
+      <c r="CJ27" s="55"/>
+      <c r="CK27" s="55"/>
+      <c r="CL27" s="55"/>
+      <c r="CM27" s="55"/>
+      <c r="CN27" s="55"/>
+      <c r="CO27" s="55"/>
+      <c r="CP27" s="55"/>
+      <c r="CQ27" s="55"/>
+      <c r="CR27" s="55"/>
+      <c r="CS27" s="55"/>
+      <c r="CT27" s="55"/>
+      <c r="CU27" s="55"/>
+      <c r="CV27" s="55"/>
+      <c r="CW27" s="55"/>
+      <c r="CX27" s="55"/>
+      <c r="CY27" s="55"/>
+      <c r="CZ27" s="55"/>
+      <c r="DA27" s="55"/>
+      <c r="DB27" s="55"/>
+      <c r="DC27" s="55"/>
+      <c r="DD27" s="55"/>
+      <c r="DE27" s="55"/>
+      <c r="DF27" s="55"/>
+      <c r="DG27" s="55"/>
+      <c r="DH27" s="55"/>
+      <c r="DI27" s="55"/>
+      <c r="DJ27" s="55"/>
+      <c r="DK27" s="55"/>
+      <c r="DL27" s="55"/>
+      <c r="DM27" s="55"/>
+    </row>
+    <row r="28" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="31" t="s">
         <v>53</v>
       </c>
@@ -3177,121 +3261,121 @@
       <c r="F28" s="34">
         <v>13</v>
       </c>
-      <c r="G28" s="80"/>
-      <c r="H28" s="85" t="s">
+      <c r="G28" s="70"/>
+      <c r="H28" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="I28" s="59"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="59"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="59"/>
-      <c r="W28" s="59"/>
-      <c r="X28" s="59"/>
-      <c r="Y28" s="59"/>
-      <c r="Z28" s="59"/>
-      <c r="AA28" s="59"/>
-      <c r="AB28" s="59"/>
-      <c r="AC28" s="59"/>
-      <c r="AD28" s="59"/>
-      <c r="AE28" s="59"/>
-      <c r="AF28" s="59"/>
-      <c r="AG28" s="59"/>
-      <c r="AH28" s="59"/>
-      <c r="AI28" s="59"/>
-      <c r="AJ28" s="59"/>
-      <c r="AK28" s="59"/>
-      <c r="AL28" s="59"/>
-      <c r="AM28" s="59"/>
-      <c r="AN28" s="59"/>
-      <c r="AO28" s="59"/>
-      <c r="AP28" s="59"/>
-      <c r="AQ28" s="59"/>
-      <c r="AR28" s="59"/>
-      <c r="AS28" s="59"/>
-      <c r="AT28" s="59"/>
-      <c r="AU28" s="59"/>
-      <c r="AV28" s="59"/>
-      <c r="AW28" s="59"/>
-      <c r="AX28" s="59"/>
-      <c r="AY28" s="59"/>
-      <c r="AZ28" s="59"/>
-      <c r="BA28" s="59"/>
-      <c r="BB28" s="59"/>
-      <c r="BC28" s="59"/>
-      <c r="BD28" s="59"/>
-      <c r="BE28" s="59"/>
-      <c r="BF28" s="59"/>
-      <c r="BG28" s="59"/>
-      <c r="BH28" s="59"/>
-      <c r="BI28" s="59"/>
-      <c r="BJ28" s="59"/>
-      <c r="BK28" s="59"/>
-      <c r="BL28" s="59"/>
-      <c r="BM28" s="59"/>
-      <c r="BN28" s="59"/>
-      <c r="BO28" s="59"/>
-      <c r="BP28" s="59"/>
-      <c r="BQ28" s="59"/>
-      <c r="BR28" s="59"/>
-      <c r="BS28" s="59"/>
-      <c r="BT28" s="59"/>
-      <c r="BU28" s="59"/>
-      <c r="BV28" s="59"/>
-      <c r="BW28" s="59"/>
-      <c r="BX28" s="59"/>
-      <c r="BY28" s="59"/>
-      <c r="BZ28" s="59"/>
-      <c r="CA28" s="59"/>
-      <c r="CB28" s="59"/>
-      <c r="CC28" s="59"/>
-      <c r="CD28" s="59"/>
-      <c r="CE28" s="59"/>
-      <c r="CF28" s="59"/>
-      <c r="CG28" s="59"/>
-      <c r="CH28" s="59"/>
-      <c r="CI28" s="59"/>
-      <c r="CJ28" s="59"/>
-      <c r="CK28" s="59"/>
-      <c r="CL28" s="59"/>
-      <c r="CM28" s="59"/>
-      <c r="CN28" s="59"/>
-      <c r="CO28" s="59"/>
-      <c r="CP28" s="59"/>
-      <c r="CQ28" s="59"/>
-      <c r="CR28" s="59"/>
-      <c r="CS28" s="59"/>
-      <c r="CT28" s="59"/>
-      <c r="CU28" s="59"/>
-      <c r="CV28" s="59"/>
-      <c r="CW28" s="59"/>
-      <c r="CX28" s="59"/>
-      <c r="CY28" s="59"/>
-      <c r="CZ28" s="59"/>
-      <c r="DA28" s="59"/>
-      <c r="DB28" s="59"/>
-      <c r="DC28" s="59"/>
-      <c r="DD28" s="59"/>
-      <c r="DE28" s="59"/>
-      <c r="DF28" s="59"/>
-      <c r="DG28" s="59"/>
-      <c r="DH28" s="59"/>
-      <c r="DI28" s="59"/>
-      <c r="DJ28" s="59"/>
-      <c r="DK28" s="59"/>
-      <c r="DL28" s="59"/>
-      <c r="DM28" s="59"/>
-    </row>
-    <row r="29" spans="1:117" s="42" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="55"/>
+      <c r="J28" s="55"/>
+      <c r="K28" s="55"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="55"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+      <c r="U28" s="55"/>
+      <c r="V28" s="55"/>
+      <c r="W28" s="55"/>
+      <c r="X28" s="55"/>
+      <c r="Y28" s="55"/>
+      <c r="Z28" s="55"/>
+      <c r="AA28" s="55"/>
+      <c r="AB28" s="55"/>
+      <c r="AC28" s="55"/>
+      <c r="AD28" s="55"/>
+      <c r="AE28" s="55"/>
+      <c r="AF28" s="55"/>
+      <c r="AG28" s="55"/>
+      <c r="AH28" s="55"/>
+      <c r="AI28" s="55"/>
+      <c r="AJ28" s="55"/>
+      <c r="AK28" s="55"/>
+      <c r="AL28" s="55"/>
+      <c r="AM28" s="55"/>
+      <c r="AN28" s="55"/>
+      <c r="AO28" s="55"/>
+      <c r="AP28" s="55"/>
+      <c r="AQ28" s="55"/>
+      <c r="AR28" s="55"/>
+      <c r="AS28" s="55"/>
+      <c r="AT28" s="55"/>
+      <c r="AU28" s="55"/>
+      <c r="AV28" s="55"/>
+      <c r="AW28" s="55"/>
+      <c r="AX28" s="55"/>
+      <c r="AY28" s="55"/>
+      <c r="AZ28" s="55"/>
+      <c r="BA28" s="55"/>
+      <c r="BB28" s="55"/>
+      <c r="BC28" s="55"/>
+      <c r="BD28" s="55"/>
+      <c r="BE28" s="55"/>
+      <c r="BF28" s="55"/>
+      <c r="BG28" s="55"/>
+      <c r="BH28" s="55"/>
+      <c r="BI28" s="55"/>
+      <c r="BJ28" s="55"/>
+      <c r="BK28" s="55"/>
+      <c r="BL28" s="55"/>
+      <c r="BM28" s="55"/>
+      <c r="BN28" s="55"/>
+      <c r="BO28" s="55"/>
+      <c r="BP28" s="55"/>
+      <c r="BQ28" s="55"/>
+      <c r="BR28" s="55"/>
+      <c r="BS28" s="55"/>
+      <c r="BT28" s="55"/>
+      <c r="BU28" s="55"/>
+      <c r="BV28" s="55"/>
+      <c r="BW28" s="55"/>
+      <c r="BX28" s="55"/>
+      <c r="BY28" s="55"/>
+      <c r="BZ28" s="55"/>
+      <c r="CA28" s="55"/>
+      <c r="CB28" s="55"/>
+      <c r="CC28" s="55"/>
+      <c r="CD28" s="55"/>
+      <c r="CE28" s="55"/>
+      <c r="CF28" s="55"/>
+      <c r="CG28" s="55"/>
+      <c r="CH28" s="55"/>
+      <c r="CI28" s="55"/>
+      <c r="CJ28" s="55"/>
+      <c r="CK28" s="55"/>
+      <c r="CL28" s="55"/>
+      <c r="CM28" s="55"/>
+      <c r="CN28" s="55"/>
+      <c r="CO28" s="55"/>
+      <c r="CP28" s="55"/>
+      <c r="CQ28" s="55"/>
+      <c r="CR28" s="55"/>
+      <c r="CS28" s="55"/>
+      <c r="CT28" s="55"/>
+      <c r="CU28" s="55"/>
+      <c r="CV28" s="55"/>
+      <c r="CW28" s="55"/>
+      <c r="CX28" s="55"/>
+      <c r="CY28" s="55"/>
+      <c r="CZ28" s="55"/>
+      <c r="DA28" s="55"/>
+      <c r="DB28" s="55"/>
+      <c r="DC28" s="55"/>
+      <c r="DD28" s="55"/>
+      <c r="DE28" s="55"/>
+      <c r="DF28" s="55"/>
+      <c r="DG28" s="55"/>
+      <c r="DH28" s="55"/>
+      <c r="DI28" s="55"/>
+      <c r="DJ28" s="55"/>
+      <c r="DK28" s="55"/>
+      <c r="DL28" s="55"/>
+      <c r="DM28" s="55"/>
+    </row>
+    <row r="29" spans="1:117" s="38" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="31" t="s">
         <v>54</v>
       </c>
@@ -3314,121 +3398,121 @@
       <c r="H29" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-      <c r="R29" s="59"/>
-      <c r="S29" s="59"/>
-      <c r="T29" s="59"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="59"/>
-      <c r="W29" s="59"/>
-      <c r="X29" s="59"/>
-      <c r="Y29" s="59"/>
-      <c r="Z29" s="59"/>
-      <c r="AA29" s="59"/>
-      <c r="AB29" s="59"/>
-      <c r="AC29" s="59"/>
-      <c r="AD29" s="59"/>
-      <c r="AE29" s="59"/>
-      <c r="AF29" s="59"/>
-      <c r="AG29" s="59"/>
-      <c r="AH29" s="59"/>
-      <c r="AI29" s="59"/>
-      <c r="AJ29" s="59"/>
-      <c r="AK29" s="59"/>
-      <c r="AL29" s="59"/>
-      <c r="AM29" s="59"/>
-      <c r="AN29" s="59"/>
-      <c r="AO29" s="59"/>
-      <c r="AP29" s="59"/>
-      <c r="AQ29" s="59"/>
-      <c r="AR29" s="59"/>
-      <c r="AS29" s="59"/>
-      <c r="AT29" s="59"/>
-      <c r="AU29" s="59"/>
-      <c r="AV29" s="59"/>
-      <c r="AW29" s="59"/>
-      <c r="AX29" s="59"/>
-      <c r="AY29" s="59"/>
-      <c r="AZ29" s="59"/>
-      <c r="BA29" s="59"/>
-      <c r="BB29" s="59"/>
-      <c r="BC29" s="59"/>
-      <c r="BD29" s="59"/>
-      <c r="BE29" s="59"/>
-      <c r="BF29" s="59"/>
-      <c r="BG29" s="59"/>
-      <c r="BH29" s="59"/>
-      <c r="BI29" s="59"/>
-      <c r="BJ29" s="59"/>
-      <c r="BK29" s="59"/>
-      <c r="BL29" s="59"/>
-      <c r="BM29" s="59"/>
-      <c r="BN29" s="59"/>
-      <c r="BO29" s="59"/>
-      <c r="BP29" s="59"/>
-      <c r="BQ29" s="59"/>
-      <c r="BR29" s="59"/>
-      <c r="BS29" s="59"/>
-      <c r="BT29" s="59"/>
-      <c r="BU29" s="59"/>
-      <c r="BV29" s="59"/>
-      <c r="BW29" s="59"/>
-      <c r="BX29" s="59"/>
-      <c r="BY29" s="59"/>
-      <c r="BZ29" s="59"/>
-      <c r="CA29" s="59"/>
-      <c r="CB29" s="59"/>
-      <c r="CC29" s="59"/>
-      <c r="CD29" s="59"/>
-      <c r="CE29" s="59"/>
-      <c r="CF29" s="59"/>
-      <c r="CG29" s="59"/>
-      <c r="CH29" s="59"/>
-      <c r="CI29" s="59"/>
-      <c r="CJ29" s="59"/>
-      <c r="CK29" s="59"/>
-      <c r="CL29" s="59"/>
-      <c r="CM29" s="59"/>
-      <c r="CN29" s="59"/>
-      <c r="CO29" s="59"/>
-      <c r="CP29" s="59"/>
-      <c r="CQ29" s="59"/>
-      <c r="CR29" s="59"/>
-      <c r="CS29" s="59"/>
-      <c r="CT29" s="59"/>
-      <c r="CU29" s="59"/>
-      <c r="CV29" s="59"/>
-      <c r="CW29" s="59"/>
-      <c r="CX29" s="59"/>
-      <c r="CY29" s="59"/>
-      <c r="CZ29" s="59"/>
-      <c r="DA29" s="59"/>
-      <c r="DB29" s="59"/>
-      <c r="DC29" s="59"/>
-      <c r="DD29" s="59"/>
-      <c r="DE29" s="59"/>
-      <c r="DF29" s="59"/>
-      <c r="DG29" s="59"/>
-      <c r="DH29" s="59"/>
-      <c r="DI29" s="59"/>
-      <c r="DJ29" s="59"/>
-      <c r="DK29" s="59"/>
-      <c r="DL29" s="59"/>
-      <c r="DM29" s="59"/>
-    </row>
-    <row r="30" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="55"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="55"/>
+      <c r="V29" s="55"/>
+      <c r="W29" s="55"/>
+      <c r="X29" s="55"/>
+      <c r="Y29" s="55"/>
+      <c r="Z29" s="55"/>
+      <c r="AA29" s="55"/>
+      <c r="AB29" s="55"/>
+      <c r="AC29" s="55"/>
+      <c r="AD29" s="55"/>
+      <c r="AE29" s="55"/>
+      <c r="AF29" s="55"/>
+      <c r="AG29" s="55"/>
+      <c r="AH29" s="55"/>
+      <c r="AI29" s="55"/>
+      <c r="AJ29" s="55"/>
+      <c r="AK29" s="55"/>
+      <c r="AL29" s="55"/>
+      <c r="AM29" s="55"/>
+      <c r="AN29" s="55"/>
+      <c r="AO29" s="55"/>
+      <c r="AP29" s="55"/>
+      <c r="AQ29" s="55"/>
+      <c r="AR29" s="55"/>
+      <c r="AS29" s="55"/>
+      <c r="AT29" s="55"/>
+      <c r="AU29" s="55"/>
+      <c r="AV29" s="55"/>
+      <c r="AW29" s="55"/>
+      <c r="AX29" s="55"/>
+      <c r="AY29" s="55"/>
+      <c r="AZ29" s="55"/>
+      <c r="BA29" s="55"/>
+      <c r="BB29" s="55"/>
+      <c r="BC29" s="55"/>
+      <c r="BD29" s="55"/>
+      <c r="BE29" s="55"/>
+      <c r="BF29" s="55"/>
+      <c r="BG29" s="55"/>
+      <c r="BH29" s="55"/>
+      <c r="BI29" s="55"/>
+      <c r="BJ29" s="55"/>
+      <c r="BK29" s="55"/>
+      <c r="BL29" s="55"/>
+      <c r="BM29" s="55"/>
+      <c r="BN29" s="55"/>
+      <c r="BO29" s="55"/>
+      <c r="BP29" s="55"/>
+      <c r="BQ29" s="55"/>
+      <c r="BR29" s="55"/>
+      <c r="BS29" s="55"/>
+      <c r="BT29" s="55"/>
+      <c r="BU29" s="55"/>
+      <c r="BV29" s="55"/>
+      <c r="BW29" s="55"/>
+      <c r="BX29" s="55"/>
+      <c r="BY29" s="55"/>
+      <c r="BZ29" s="55"/>
+      <c r="CA29" s="55"/>
+      <c r="CB29" s="55"/>
+      <c r="CC29" s="55"/>
+      <c r="CD29" s="55"/>
+      <c r="CE29" s="55"/>
+      <c r="CF29" s="55"/>
+      <c r="CG29" s="55"/>
+      <c r="CH29" s="55"/>
+      <c r="CI29" s="55"/>
+      <c r="CJ29" s="55"/>
+      <c r="CK29" s="55"/>
+      <c r="CL29" s="55"/>
+      <c r="CM29" s="55"/>
+      <c r="CN29" s="55"/>
+      <c r="CO29" s="55"/>
+      <c r="CP29" s="55"/>
+      <c r="CQ29" s="55"/>
+      <c r="CR29" s="55"/>
+      <c r="CS29" s="55"/>
+      <c r="CT29" s="55"/>
+      <c r="CU29" s="55"/>
+      <c r="CV29" s="55"/>
+      <c r="CW29" s="55"/>
+      <c r="CX29" s="55"/>
+      <c r="CY29" s="55"/>
+      <c r="CZ29" s="55"/>
+      <c r="DA29" s="55"/>
+      <c r="DB29" s="55"/>
+      <c r="DC29" s="55"/>
+      <c r="DD29" s="55"/>
+      <c r="DE29" s="55"/>
+      <c r="DF29" s="55"/>
+      <c r="DG29" s="55"/>
+      <c r="DH29" s="55"/>
+      <c r="DI29" s="55"/>
+      <c r="DJ29" s="55"/>
+      <c r="DK29" s="55"/>
+      <c r="DL29" s="55"/>
+      <c r="DM29" s="55"/>
+    </row>
+    <row r="30" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="50" t="s">
         <v>74</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -3443,12 +3527,12 @@
       <c r="F30" s="12">
         <v>5</v>
       </c>
-      <c r="G30" s="79"/>
+      <c r="G30" s="69"/>
       <c r="H30" s="35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="31" t="s">
         <v>60</v>
       </c>
@@ -3474,7 +3558,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:117" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="31" t="s">
         <v>59</v>
       </c>
@@ -3500,79 +3584,214 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+    <row r="33" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40" t="s">
+      <c r="B33" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="74" t="s">
+      <c r="E33" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F33" s="68">
+      <c r="F33" s="66">
         <v>13</v>
       </c>
-      <c r="G33" s="81">
+      <c r="G33" s="79">
         <v>19</v>
       </c>
-      <c r="H33" s="41" t="s">
+      <c r="H33" s="80" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
+    <row r="34" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="71" t="s">
+      <c r="B34" s="82" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="68" t="s">
+      <c r="D34" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="74" t="s">
+      <c r="E34" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="68">
+      <c r="F34" s="66">
         <v>13</v>
       </c>
-      <c r="G34" s="66">
+      <c r="G34" s="84">
         <v>24</v>
       </c>
-      <c r="H34" s="83" t="s">
+      <c r="H34" s="85" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="68" t="s">
+    <row r="35" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="66"/>
-      <c r="C35" s="68" t="s">
+      <c r="B35" s="84"/>
+      <c r="C35" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="68" t="s">
+      <c r="D35" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="74" t="s">
+      <c r="E35" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="68">
+      <c r="F35" s="66">
         <v>13</v>
       </c>
-      <c r="G35" s="66">
+      <c r="G35" s="84">
         <v>27</v>
       </c>
-      <c r="H35" s="84" t="s">
+      <c r="H35" s="86" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="87" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="87">
+        <v>8</v>
+      </c>
+      <c r="G36" s="87">
+        <v>31</v>
+      </c>
+      <c r="H36" s="88" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="89" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="87">
+        <v>13</v>
+      </c>
+      <c r="G37" s="87">
+        <v>30</v>
+      </c>
+      <c r="H37" s="52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="89" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="90" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="87" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="87">
+        <v>13</v>
+      </c>
+      <c r="G38" s="87">
+        <v>29</v>
+      </c>
+      <c r="H38" s="52" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="91"/>
+      <c r="C39" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="87">
+        <v>21</v>
+      </c>
+      <c r="G39" s="87">
+        <v>32</v>
+      </c>
+      <c r="H39" s="36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="93"/>
+      <c r="B40" s="93"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="93"/>
+      <c r="H40" s="94"/>
+    </row>
+    <row r="41" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="93"/>
+      <c r="B41" s="93"/>
+      <c r="C41" s="93"/>
+      <c r="D41" s="93"/>
+      <c r="E41" s="93"/>
+      <c r="F41" s="93"/>
+      <c r="G41" s="93"/>
+      <c r="H41" s="94"/>
+    </row>
+    <row r="42" spans="1:8" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="93"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="93"/>
+      <c r="H42" s="94"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>

</xml_diff>